<commit_message>
monday work? not sure
</commit_message>
<xml_diff>
--- a/bundle_slat_characterization/GRIPS Bundle Sequence.xlsx
+++ b/bundle_slat_characterization/GRIPS Bundle Sequence.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23812"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="36540" windowHeight="23560" tabRatio="944" firstSheet="17" activeTab="39"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="36560" windowHeight="23560" tabRatio="944" firstSheet="17" activeTab="39"/>
   </bookViews>
   <sheets>
     <sheet name="A" sheetId="1" r:id="rId1"/>
@@ -859,9 +859,6 @@
     <t>bb</t>
   </si>
   <si>
-    <t>pinching between this slat and the one below</t>
-  </si>
-  <si>
     <t>see legend to right</t>
   </si>
   <si>
@@ -877,7 +874,10 @@
     <t>upside down =flip  top-bottom</t>
   </si>
   <si>
-    <t xml:space="preserve">Bundles are organized so that the bottom of a bundle (denoted with slamp at bottom) is towards the outer ring of the mask. </t>
+    <t>pinching between the bottom slat of this bundle and the top slat of the one below</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bundles are organized so that the bottom of a bundle (denoted with letter and number at bottom) is towards the outer ring of the mask. </t>
   </si>
 </sst>
 </file>
@@ -2171,6 +2171,7 @@
     <xf numFmtId="0" fontId="18" fillId="8" borderId="21" xfId="65" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="6" borderId="22" xfId="65" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="6" borderId="23" xfId="65" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2186,6 +2187,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2193,9 +2197,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="4" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2213,7 +2214,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="66">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2323,7 +2323,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2409,11 +2408,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2086682488"/>
-        <c:axId val="2086675320"/>
+        <c:axId val="2072034808"/>
+        <c:axId val="2094147704"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2086682488"/>
+        <c:axId val="2072034808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2440,13 +2439,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2086675320"/>
+        <c:crossAx val="2094147704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2454,7 +2452,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2086675320"/>
+        <c:axId val="2094147704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2476,14 +2474,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2086682488"/>
+        <c:crossAx val="2072034808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2680,11 +2677,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2129818184"/>
-        <c:axId val="-2129812504"/>
+        <c:axId val="2094653032"/>
+        <c:axId val="2094658712"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2129818184"/>
+        <c:axId val="2094653032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2716,7 +2713,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2129812504"/>
+        <c:crossAx val="2094658712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2724,7 +2721,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2129812504"/>
+        <c:axId val="2094658712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2752,7 +2749,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2129818184"/>
+        <c:crossAx val="2094653032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2949,11 +2946,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2129771672"/>
-        <c:axId val="-2129765992"/>
+        <c:axId val="2094699544"/>
+        <c:axId val="2094705224"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2129771672"/>
+        <c:axId val="2094699544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2985,7 +2982,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2129765992"/>
+        <c:crossAx val="2094705224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2993,7 +2990,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2129765992"/>
+        <c:axId val="2094705224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3021,7 +3018,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2129771672"/>
+        <c:crossAx val="2094699544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3218,11 +3215,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2129712696"/>
-        <c:axId val="-2129707256"/>
+        <c:axId val="2094754312"/>
+        <c:axId val="2094759752"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2129712696"/>
+        <c:axId val="2094754312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3249,7 +3246,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2129707256"/>
+        <c:crossAx val="2094759752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3257,7 +3254,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2129707256"/>
+        <c:axId val="2094759752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3285,7 +3282,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2129712696"/>
+        <c:crossAx val="2094754312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3482,11 +3479,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2130388136"/>
-        <c:axId val="-2130393832"/>
+        <c:axId val="2094800152"/>
+        <c:axId val="2094805832"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2130388136"/>
+        <c:axId val="2094800152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3518,7 +3515,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2130393832"/>
+        <c:crossAx val="2094805832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3526,7 +3523,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2130393832"/>
+        <c:axId val="2094805832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3554,7 +3551,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2130388136"/>
+        <c:crossAx val="2094800152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3606,7 +3603,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3722,11 +3718,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2130441592"/>
-        <c:axId val="-2130447352"/>
+        <c:axId val="2094853672"/>
+        <c:axId val="2094859416"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2130441592"/>
+        <c:axId val="2094853672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3753,13 +3749,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2130447352"/>
+        <c:crossAx val="2094859416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3767,7 +3762,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2130447352"/>
+        <c:axId val="2094859416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3789,14 +3784,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2130441592"/>
+        <c:crossAx val="2094853672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3963,11 +3957,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2130487960"/>
-        <c:axId val="-2130493720"/>
+        <c:axId val="2094900024"/>
+        <c:axId val="2094905768"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2130487960"/>
+        <c:axId val="2094900024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3999,7 +3993,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2130493720"/>
+        <c:crossAx val="2094905768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4007,7 +4001,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2130493720"/>
+        <c:axId val="2094905768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4035,7 +4029,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2130487960"/>
+        <c:crossAx val="2094900024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4256,11 +4250,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2130547864"/>
-        <c:axId val="-2130553560"/>
+        <c:axId val="2094959960"/>
+        <c:axId val="2094965640"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2130547864"/>
+        <c:axId val="2094959960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4292,7 +4286,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2130553560"/>
+        <c:crossAx val="2094965640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4300,7 +4294,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2130553560"/>
+        <c:axId val="2094965640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4328,7 +4322,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2130547864"/>
+        <c:crossAx val="2094959960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4507,11 +4501,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2130603400"/>
-        <c:axId val="-2130609160"/>
+        <c:axId val="2095015480"/>
+        <c:axId val="2095021224"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2130603400"/>
+        <c:axId val="2095015480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4543,7 +4537,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2130609160"/>
+        <c:crossAx val="2095021224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4551,7 +4545,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2130609160"/>
+        <c:axId val="2095021224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4579,7 +4573,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2130603400"/>
+        <c:crossAx val="2095015480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4794,11 +4788,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2130660312"/>
-        <c:axId val="-2130666008"/>
+        <c:axId val="2094111272"/>
+        <c:axId val="2094105576"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2130660312"/>
+        <c:axId val="2094111272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4830,7 +4824,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2130666008"/>
+        <c:crossAx val="2094105576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4838,7 +4832,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2130666008"/>
+        <c:axId val="2094105576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4866,7 +4860,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2130660312"/>
+        <c:crossAx val="2094111272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5081,11 +5075,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2129330040"/>
-        <c:axId val="-2129324360"/>
+        <c:axId val="2094062904"/>
+        <c:axId val="2094057208"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2129330040"/>
+        <c:axId val="2094062904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5117,7 +5111,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2129324360"/>
+        <c:crossAx val="2094057208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5125,7 +5119,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2129324360"/>
+        <c:axId val="2094057208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5153,7 +5147,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2129330040"/>
+        <c:crossAx val="2094062904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5205,7 +5199,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -5291,11 +5284,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2130313352"/>
-        <c:axId val="-2130307896"/>
+        <c:axId val="2093090104"/>
+        <c:axId val="2093084616"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2130313352"/>
+        <c:axId val="2093090104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5317,13 +5310,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2130307896"/>
+        <c:crossAx val="2093084616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5331,7 +5323,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2130307896"/>
+        <c:axId val="2093084616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5353,14 +5345,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2130313352"/>
+        <c:crossAx val="2093090104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5412,7 +5403,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -5522,11 +5512,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2130225048"/>
-        <c:axId val="-2130219304"/>
+        <c:axId val="2094245416"/>
+        <c:axId val="2094251176"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2130225048"/>
+        <c:axId val="2094245416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5553,13 +5543,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2130219304"/>
+        <c:crossAx val="2094251176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5567,7 +5556,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2130219304"/>
+        <c:axId val="2094251176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5589,14 +5578,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2130225048"/>
+        <c:crossAx val="2094245416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5643,7 +5631,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -5753,11 +5740,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2130160696"/>
-        <c:axId val="-2130154952"/>
+        <c:axId val="2094309768"/>
+        <c:axId val="2094315512"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2130160696"/>
+        <c:axId val="2094309768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5784,13 +5771,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2130154952"/>
+        <c:crossAx val="2094315512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5798,7 +5784,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2130154952"/>
+        <c:axId val="2094315512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5820,14 +5806,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2130160696"/>
+        <c:crossAx val="2094309768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5879,7 +5864,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -5989,11 +5973,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2130103416"/>
-        <c:axId val="-2130097672"/>
+        <c:axId val="2094367624"/>
+        <c:axId val="2094373368"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2130103416"/>
+        <c:axId val="2094367624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6020,13 +6004,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2130097672"/>
+        <c:crossAx val="2094373368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6034,7 +6017,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2130097672"/>
+        <c:axId val="2094373368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6056,14 +6039,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2130103416"/>
+        <c:crossAx val="2094367624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6224,11 +6206,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2130057352"/>
-        <c:axId val="-2130051608"/>
+        <c:axId val="2094413688"/>
+        <c:axId val="2094419432"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2130057352"/>
+        <c:axId val="2094413688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6260,7 +6242,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2130051608"/>
+        <c:crossAx val="2094419432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6268,7 +6250,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2130051608"/>
+        <c:axId val="2094419432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6296,7 +6278,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2130057352"/>
+        <c:crossAx val="2094413688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6457,11 +6439,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2129989384"/>
-        <c:axId val="-2129983640"/>
+        <c:axId val="2094481656"/>
+        <c:axId val="2094487400"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2129989384"/>
+        <c:axId val="2094481656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6493,7 +6475,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2129983640"/>
+        <c:crossAx val="2094487400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6501,7 +6483,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2129983640"/>
+        <c:axId val="2094487400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6529,7 +6511,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2129989384"/>
+        <c:crossAx val="2094481656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6696,11 +6678,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2129926600"/>
-        <c:axId val="-2129920856"/>
+        <c:axId val="2094544520"/>
+        <c:axId val="2094550264"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2129926600"/>
+        <c:axId val="2094544520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6732,7 +6714,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2129920856"/>
+        <c:crossAx val="2094550264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6740,7 +6722,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2129920856"/>
+        <c:axId val="2094550264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6768,7 +6750,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2129926600"/>
+        <c:crossAx val="2094544520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6935,11 +6917,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2129877816"/>
-        <c:axId val="-2129872072"/>
+        <c:axId val="2094593304"/>
+        <c:axId val="2094599048"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2129877816"/>
+        <c:axId val="2094593304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6971,7 +6953,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2129872072"/>
+        <c:crossAx val="2094599048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6979,7 +6961,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2129872072"/>
+        <c:axId val="2094599048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7007,7 +6989,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2129877816"/>
+        <c:crossAx val="2094593304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8328,28 +8310,28 @@
       <c r="B9" s="76" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="385" t="s">
+      <c r="C9" s="386" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="386"/>
-      <c r="E9" s="384" t="s">
+      <c r="D9" s="387"/>
+      <c r="E9" s="385" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="384"/>
-      <c r="G9" s="384"/>
-      <c r="H9" s="384"/>
-      <c r="I9" s="384"/>
+      <c r="F9" s="385"/>
+      <c r="G9" s="385"/>
+      <c r="H9" s="385"/>
+      <c r="I9" s="385"/>
       <c r="J9" s="75"/>
-      <c r="K9" s="385" t="s">
+      <c r="K9" s="386" t="s">
         <v>38</v>
       </c>
-      <c r="L9" s="386"/>
-      <c r="M9" s="383" t="s">
+      <c r="L9" s="387"/>
+      <c r="M9" s="384" t="s">
         <v>37</v>
       </c>
-      <c r="N9" s="383"/>
-      <c r="O9" s="383"/>
-      <c r="P9" s="383"/>
+      <c r="N9" s="384"/>
+      <c r="O9" s="384"/>
+      <c r="P9" s="384"/>
       <c r="Q9" s="74" t="s">
         <v>36</v>
       </c>
@@ -12611,34 +12593,34 @@
         <v>17</v>
       </c>
       <c r="B68" s="1"/>
-      <c r="C68" s="382" t="s">
+      <c r="C68" s="383" t="s">
         <v>16</v>
       </c>
-      <c r="D68" s="382"/>
-      <c r="E68" s="382" t="s">
+      <c r="D68" s="383"/>
+      <c r="E68" s="383" t="s">
         <v>15</v>
       </c>
-      <c r="F68" s="382"/>
+      <c r="F68" s="383"/>
       <c r="G68" s="1"/>
       <c r="H68" s="1"/>
       <c r="I68" s="1"/>
       <c r="J68" s="1"/>
-      <c r="K68" s="382" t="s">
+      <c r="K68" s="383" t="s">
         <v>14</v>
       </c>
-      <c r="L68" s="382"/>
+      <c r="L68" s="383"/>
       <c r="M68" s="1"/>
       <c r="N68" s="1"/>
       <c r="O68" s="1"/>
       <c r="P68" s="1"/>
-      <c r="Q68" s="382" t="s">
+      <c r="Q68" s="383" t="s">
         <v>13</v>
       </c>
-      <c r="R68" s="382"/>
-      <c r="S68" s="382" t="s">
+      <c r="R68" s="383"/>
+      <c r="S68" s="383" t="s">
         <v>12</v>
       </c>
-      <c r="T68" s="382"/>
+      <c r="T68" s="383"/>
       <c r="U68" s="1"/>
       <c r="V68" s="1"/>
       <c r="W68" s="1"/>
@@ -13682,28 +13664,28 @@
       <c r="B9" s="261" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="385" t="s">
+      <c r="C9" s="386" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="386"/>
-      <c r="E9" s="384" t="s">
+      <c r="D9" s="387"/>
+      <c r="E9" s="385" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="384"/>
-      <c r="G9" s="384"/>
-      <c r="H9" s="384"/>
-      <c r="I9" s="384"/>
+      <c r="F9" s="385"/>
+      <c r="G9" s="385"/>
+      <c r="H9" s="385"/>
+      <c r="I9" s="385"/>
       <c r="J9" s="75"/>
-      <c r="K9" s="385" t="s">
+      <c r="K9" s="386" t="s">
         <v>38</v>
       </c>
-      <c r="L9" s="386"/>
-      <c r="M9" s="385" t="s">
+      <c r="L9" s="387"/>
+      <c r="M9" s="386" t="s">
         <v>37</v>
       </c>
-      <c r="N9" s="383"/>
-      <c r="O9" s="383"/>
-      <c r="P9" s="383"/>
+      <c r="N9" s="384"/>
+      <c r="O9" s="384"/>
+      <c r="P9" s="384"/>
       <c r="Q9" s="74" t="s">
         <v>36</v>
       </c>
@@ -16415,28 +16397,28 @@
       <c r="B9" s="261" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="385" t="s">
+      <c r="C9" s="386" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="386"/>
-      <c r="E9" s="384" t="s">
+      <c r="D9" s="387"/>
+      <c r="E9" s="385" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="384"/>
-      <c r="G9" s="384"/>
-      <c r="H9" s="384"/>
-      <c r="I9" s="384"/>
+      <c r="F9" s="385"/>
+      <c r="G9" s="385"/>
+      <c r="H9" s="385"/>
+      <c r="I9" s="385"/>
       <c r="J9" s="75"/>
-      <c r="K9" s="385" t="s">
+      <c r="K9" s="386" t="s">
         <v>38</v>
       </c>
-      <c r="L9" s="386"/>
-      <c r="M9" s="385" t="s">
+      <c r="L9" s="387"/>
+      <c r="M9" s="386" t="s">
         <v>37</v>
       </c>
-      <c r="N9" s="383"/>
-      <c r="O9" s="383"/>
-      <c r="P9" s="383"/>
+      <c r="N9" s="384"/>
+      <c r="O9" s="384"/>
+      <c r="P9" s="384"/>
       <c r="Q9" s="74" t="s">
         <v>36</v>
       </c>
@@ -18423,28 +18405,28 @@
       <c r="B9" s="261" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="385" t="s">
+      <c r="C9" s="386" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="386"/>
-      <c r="E9" s="384" t="s">
+      <c r="D9" s="387"/>
+      <c r="E9" s="385" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="384"/>
-      <c r="G9" s="384"/>
-      <c r="H9" s="384"/>
-      <c r="I9" s="384"/>
+      <c r="F9" s="385"/>
+      <c r="G9" s="385"/>
+      <c r="H9" s="385"/>
+      <c r="I9" s="385"/>
       <c r="J9" s="75"/>
-      <c r="K9" s="385" t="s">
+      <c r="K9" s="386" t="s">
         <v>38</v>
       </c>
-      <c r="L9" s="386"/>
-      <c r="M9" s="385" t="s">
+      <c r="L9" s="387"/>
+      <c r="M9" s="386" t="s">
         <v>37</v>
       </c>
-      <c r="N9" s="383"/>
-      <c r="O9" s="383"/>
-      <c r="P9" s="383"/>
+      <c r="N9" s="384"/>
+      <c r="O9" s="384"/>
+      <c r="P9" s="384"/>
       <c r="Q9" s="74" t="s">
         <v>36</v>
       </c>
@@ -21017,28 +20999,28 @@
       <c r="B9" s="76" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="385" t="s">
+      <c r="C9" s="386" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="386"/>
-      <c r="E9" s="384" t="s">
+      <c r="D9" s="387"/>
+      <c r="E9" s="385" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="384"/>
-      <c r="G9" s="384"/>
-      <c r="H9" s="384"/>
-      <c r="I9" s="384"/>
+      <c r="F9" s="385"/>
+      <c r="G9" s="385"/>
+      <c r="H9" s="385"/>
+      <c r="I9" s="385"/>
       <c r="J9" s="75"/>
-      <c r="K9" s="385" t="s">
+      <c r="K9" s="386" t="s">
         <v>38</v>
       </c>
-      <c r="L9" s="386"/>
-      <c r="M9" s="385" t="s">
+      <c r="L9" s="387"/>
+      <c r="M9" s="386" t="s">
         <v>37</v>
       </c>
-      <c r="N9" s="383"/>
-      <c r="O9" s="383"/>
-      <c r="P9" s="383"/>
+      <c r="N9" s="384"/>
+      <c r="O9" s="384"/>
+      <c r="P9" s="384"/>
       <c r="Q9" s="74" t="s">
         <v>36</v>
       </c>
@@ -22694,28 +22676,28 @@
       <c r="B9" s="76" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="385" t="s">
+      <c r="C9" s="386" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="386"/>
-      <c r="E9" s="384" t="s">
+      <c r="D9" s="387"/>
+      <c r="E9" s="385" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="384"/>
-      <c r="G9" s="384"/>
-      <c r="H9" s="384"/>
-      <c r="I9" s="384"/>
+      <c r="F9" s="385"/>
+      <c r="G9" s="385"/>
+      <c r="H9" s="385"/>
+      <c r="I9" s="385"/>
       <c r="J9" s="75"/>
-      <c r="K9" s="385" t="s">
+      <c r="K9" s="386" t="s">
         <v>38</v>
       </c>
-      <c r="L9" s="386"/>
-      <c r="M9" s="385" t="s">
+      <c r="L9" s="387"/>
+      <c r="M9" s="386" t="s">
         <v>37</v>
       </c>
-      <c r="N9" s="383"/>
-      <c r="O9" s="383"/>
-      <c r="P9" s="383"/>
+      <c r="N9" s="384"/>
+      <c r="O9" s="384"/>
+      <c r="P9" s="384"/>
       <c r="Q9" s="74" t="s">
         <v>36</v>
       </c>
@@ -24666,28 +24648,28 @@
       <c r="B9" s="76" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="385" t="s">
+      <c r="C9" s="386" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="386"/>
-      <c r="E9" s="384" t="s">
+      <c r="D9" s="387"/>
+      <c r="E9" s="385" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="384"/>
-      <c r="G9" s="384"/>
-      <c r="H9" s="384"/>
-      <c r="I9" s="384"/>
+      <c r="F9" s="385"/>
+      <c r="G9" s="385"/>
+      <c r="H9" s="385"/>
+      <c r="I9" s="385"/>
       <c r="J9" s="75"/>
-      <c r="K9" s="385" t="s">
+      <c r="K9" s="386" t="s">
         <v>38</v>
       </c>
-      <c r="L9" s="386"/>
-      <c r="M9" s="385" t="s">
+      <c r="L9" s="387"/>
+      <c r="M9" s="386" t="s">
         <v>37</v>
       </c>
-      <c r="N9" s="383"/>
-      <c r="O9" s="383"/>
-      <c r="P9" s="383"/>
+      <c r="N9" s="384"/>
+      <c r="O9" s="384"/>
+      <c r="P9" s="384"/>
       <c r="Q9" s="74" t="s">
         <v>36</v>
       </c>
@@ -26923,28 +26905,28 @@
       <c r="B9" s="76" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="385" t="s">
+      <c r="C9" s="386" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="386"/>
-      <c r="E9" s="384" t="s">
+      <c r="D9" s="387"/>
+      <c r="E9" s="385" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="384"/>
-      <c r="G9" s="384"/>
-      <c r="H9" s="384"/>
-      <c r="I9" s="384"/>
+      <c r="F9" s="385"/>
+      <c r="G9" s="385"/>
+      <c r="H9" s="385"/>
+      <c r="I9" s="385"/>
       <c r="J9" s="75"/>
-      <c r="K9" s="385" t="s">
+      <c r="K9" s="386" t="s">
         <v>38</v>
       </c>
-      <c r="L9" s="386"/>
-      <c r="M9" s="385" t="s">
+      <c r="L9" s="387"/>
+      <c r="M9" s="386" t="s">
         <v>37</v>
       </c>
-      <c r="N9" s="383"/>
-      <c r="O9" s="383"/>
-      <c r="P9" s="383"/>
+      <c r="N9" s="384"/>
+      <c r="O9" s="384"/>
+      <c r="P9" s="384"/>
       <c r="Q9" s="74" t="s">
         <v>36</v>
       </c>
@@ -28941,28 +28923,28 @@
       <c r="B9" s="76" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="385" t="s">
+      <c r="C9" s="386" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="386"/>
-      <c r="E9" s="384" t="s">
+      <c r="D9" s="387"/>
+      <c r="E9" s="385" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="384"/>
-      <c r="G9" s="384"/>
-      <c r="H9" s="384"/>
-      <c r="I9" s="384"/>
+      <c r="F9" s="385"/>
+      <c r="G9" s="385"/>
+      <c r="H9" s="385"/>
+      <c r="I9" s="385"/>
       <c r="J9" s="75"/>
-      <c r="K9" s="385" t="s">
+      <c r="K9" s="386" t="s">
         <v>38</v>
       </c>
-      <c r="L9" s="386"/>
-      <c r="M9" s="385" t="s">
+      <c r="L9" s="387"/>
+      <c r="M9" s="386" t="s">
         <v>37</v>
       </c>
-      <c r="N9" s="383"/>
-      <c r="O9" s="383"/>
-      <c r="P9" s="383"/>
+      <c r="N9" s="384"/>
+      <c r="O9" s="384"/>
+      <c r="P9" s="384"/>
       <c r="Q9" s="74" t="s">
         <v>36</v>
       </c>
@@ -30440,28 +30422,28 @@
       <c r="B9" s="76" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="385" t="s">
+      <c r="C9" s="386" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="386"/>
-      <c r="E9" s="384" t="s">
+      <c r="D9" s="387"/>
+      <c r="E9" s="385" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="384"/>
-      <c r="G9" s="384"/>
-      <c r="H9" s="384"/>
-      <c r="I9" s="384"/>
+      <c r="F9" s="385"/>
+      <c r="G9" s="385"/>
+      <c r="H9" s="385"/>
+      <c r="I9" s="385"/>
       <c r="J9" s="75"/>
-      <c r="K9" s="385" t="s">
+      <c r="K9" s="386" t="s">
         <v>38</v>
       </c>
-      <c r="L9" s="386"/>
-      <c r="M9" s="385" t="s">
+      <c r="L9" s="387"/>
+      <c r="M9" s="386" t="s">
         <v>37</v>
       </c>
-      <c r="N9" s="383"/>
-      <c r="O9" s="383"/>
-      <c r="P9" s="383"/>
+      <c r="N9" s="384"/>
+      <c r="O9" s="384"/>
+      <c r="P9" s="384"/>
       <c r="Q9" s="74" t="s">
         <v>36</v>
       </c>
@@ -31211,10 +31193,10 @@
       <c r="C30" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D30" s="394" t="s">
+      <c r="D30" s="395" t="s">
         <v>1</v>
       </c>
-      <c r="E30" s="394"/>
+      <c r="E30" s="395"/>
       <c r="F30" s="7"/>
       <c r="G30" s="6"/>
       <c r="H30" s="6"/>
@@ -31610,10 +31592,10 @@
       <c r="N8" s="79"/>
       <c r="O8" s="79"/>
       <c r="P8" s="79"/>
-      <c r="V8" s="395" t="s">
+      <c r="V8" s="396" t="s">
         <v>42</v>
       </c>
-      <c r="W8" s="395"/>
+      <c r="W8" s="396"/>
     </row>
     <row r="9" spans="1:27" ht="30" customHeight="1">
       <c r="A9" s="71" t="s">
@@ -31622,28 +31604,28 @@
       <c r="B9" s="261" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="385" t="s">
+      <c r="C9" s="386" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="386"/>
-      <c r="E9" s="384" t="s">
+      <c r="D9" s="387"/>
+      <c r="E9" s="385" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="384"/>
-      <c r="G9" s="384"/>
-      <c r="H9" s="384"/>
-      <c r="I9" s="384"/>
+      <c r="F9" s="385"/>
+      <c r="G9" s="385"/>
+      <c r="H9" s="385"/>
+      <c r="I9" s="385"/>
       <c r="J9" s="75"/>
-      <c r="K9" s="385" t="s">
+      <c r="K9" s="386" t="s">
         <v>38</v>
       </c>
-      <c r="L9" s="386"/>
-      <c r="M9" s="385" t="s">
+      <c r="L9" s="387"/>
+      <c r="M9" s="386" t="s">
         <v>37</v>
       </c>
-      <c r="N9" s="383"/>
-      <c r="O9" s="383"/>
-      <c r="P9" s="383"/>
+      <c r="N9" s="384"/>
+      <c r="O9" s="384"/>
+      <c r="P9" s="384"/>
       <c r="Q9" s="74" t="s">
         <v>36</v>
       </c>
@@ -32414,10 +32396,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27">
-      <c r="A1" s="390" t="s">
+      <c r="A1" s="388" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="390"/>
+      <c r="B1" s="388"/>
       <c r="C1" s="145"/>
       <c r="D1" s="145"/>
       <c r="E1" s="146"/>
@@ -32436,10 +32418,10 @@
       <c r="T1" s="144"/>
     </row>
     <row r="2" spans="1:27">
-      <c r="A2" s="390" t="s">
+      <c r="A2" s="388" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="390"/>
+      <c r="B2" s="388"/>
       <c r="C2" s="145"/>
       <c r="D2" s="145"/>
       <c r="E2" s="146"/>
@@ -32458,10 +32440,10 @@
       <c r="T2" s="144"/>
     </row>
     <row r="3" spans="1:27">
-      <c r="A3" s="390" t="s">
+      <c r="A3" s="388" t="s">
         <v>47</v>
       </c>
-      <c r="B3" s="390"/>
+      <c r="B3" s="388"/>
       <c r="C3" s="145"/>
       <c r="D3" s="145"/>
       <c r="E3" s="146"/>
@@ -32599,28 +32581,28 @@
       <c r="B9" s="142" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="391" t="s">
+      <c r="C9" s="392" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="392"/>
-      <c r="E9" s="393" t="s">
+      <c r="D9" s="393"/>
+      <c r="E9" s="394" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="393"/>
-      <c r="G9" s="393"/>
-      <c r="H9" s="393"/>
-      <c r="I9" s="393"/>
+      <c r="F9" s="394"/>
+      <c r="G9" s="394"/>
+      <c r="H9" s="394"/>
+      <c r="I9" s="394"/>
       <c r="J9" s="141"/>
-      <c r="K9" s="391" t="s">
+      <c r="K9" s="392" t="s">
         <v>38</v>
       </c>
-      <c r="L9" s="392"/>
-      <c r="M9" s="387" t="s">
+      <c r="L9" s="393"/>
+      <c r="M9" s="389" t="s">
         <v>37</v>
       </c>
-      <c r="N9" s="387"/>
-      <c r="O9" s="387"/>
-      <c r="P9" s="387"/>
+      <c r="N9" s="389"/>
+      <c r="O9" s="389"/>
+      <c r="P9" s="389"/>
       <c r="Q9" s="140" t="s">
         <v>53</v>
       </c>
@@ -34744,18 +34726,18 @@
         <v>16</v>
       </c>
       <c r="D43" s="23"/>
-      <c r="E43" s="388" t="s">
+      <c r="E43" s="390" t="s">
         <v>15</v>
       </c>
-      <c r="F43" s="388"/>
+      <c r="F43" s="390"/>
       <c r="G43" s="28"/>
       <c r="H43" s="28"/>
       <c r="I43" s="28"/>
       <c r="J43" s="28"/>
-      <c r="K43" s="389" t="s">
+      <c r="K43" s="391" t="s">
         <v>14</v>
       </c>
-      <c r="L43" s="389"/>
+      <c r="L43" s="391"/>
       <c r="M43" s="25"/>
       <c r="N43" s="25"/>
       <c r="O43" s="24"/>
@@ -35564,16 +35546,16 @@
     </row>
     <row r="68" spans="1:22">
       <c r="A68" s="13"/>
-      <c r="C68" s="390"/>
-      <c r="D68" s="390"/>
-      <c r="E68" s="390"/>
-      <c r="F68" s="390"/>
-      <c r="K68" s="390"/>
-      <c r="L68" s="390"/>
-      <c r="Q68" s="390"/>
-      <c r="R68" s="390"/>
-      <c r="S68" s="390"/>
-      <c r="T68" s="390"/>
+      <c r="C68" s="388"/>
+      <c r="D68" s="388"/>
+      <c r="E68" s="388"/>
+      <c r="F68" s="388"/>
+      <c r="K68" s="388"/>
+      <c r="L68" s="388"/>
+      <c r="Q68" s="388"/>
+      <c r="R68" s="388"/>
+      <c r="S68" s="388"/>
+      <c r="T68" s="388"/>
     </row>
     <row r="69" spans="1:22">
       <c r="A69" s="87"/>
@@ -35624,11 +35606,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="E68:F68"/>
-    <mergeCell ref="K68:L68"/>
-    <mergeCell ref="Q68:R68"/>
-    <mergeCell ref="S68:T68"/>
     <mergeCell ref="M9:P9"/>
     <mergeCell ref="E43:F43"/>
     <mergeCell ref="K43:L43"/>
@@ -35638,6 +35615,11 @@
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="E9:I9"/>
     <mergeCell ref="K9:L9"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="E68:F68"/>
+    <mergeCell ref="K68:L68"/>
+    <mergeCell ref="Q68:R68"/>
+    <mergeCell ref="S68:T68"/>
   </mergeCells>
   <phoneticPr fontId="16" type="noConversion"/>
   <pageMargins left="0.2" right="0.2" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
@@ -36386,12 +36368,12 @@
         <v>126</v>
       </c>
       <c r="F59" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="60" spans="1:7">
       <c r="F60" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="62" spans="1:7">
@@ -36428,7 +36410,7 @@
     </row>
     <row r="70" spans="3:4">
       <c r="C70" s="322" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D70" s="125"/>
     </row>
@@ -36469,8 +36451,8 @@
       <c r="D79" s="125"/>
     </row>
     <row r="80" spans="3:4">
-      <c r="C80" s="396" t="s">
-        <v>267</v>
+      <c r="C80" s="382" t="s">
+        <v>266</v>
       </c>
       <c r="D80" s="140"/>
     </row>
@@ -41746,10 +41728,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34">
-      <c r="A1" s="382" t="s">
+      <c r="A1" s="383" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="382"/>
+      <c r="B1" s="383"/>
       <c r="C1" s="79"/>
       <c r="D1" s="79"/>
       <c r="E1" s="80"/>
@@ -41783,10 +41765,10 @@
       <c r="AH1" s="1"/>
     </row>
     <row r="2" spans="1:34">
-      <c r="A2" s="382" t="s">
+      <c r="A2" s="383" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="382"/>
+      <c r="B2" s="383"/>
       <c r="C2" s="79"/>
       <c r="D2" s="79"/>
       <c r="E2" s="80"/>
@@ -41820,10 +41802,10 @@
       <c r="AH2" s="1"/>
     </row>
     <row r="3" spans="1:34">
-      <c r="A3" s="382" t="s">
+      <c r="A3" s="383" t="s">
         <v>47</v>
       </c>
-      <c r="B3" s="382"/>
+      <c r="B3" s="383"/>
       <c r="C3" s="79"/>
       <c r="D3" s="79"/>
       <c r="E3" s="80"/>
@@ -42052,28 +42034,28 @@
       <c r="B9" s="76" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="385" t="s">
+      <c r="C9" s="386" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="386"/>
-      <c r="E9" s="384" t="s">
+      <c r="D9" s="387"/>
+      <c r="E9" s="385" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="384"/>
-      <c r="G9" s="384"/>
-      <c r="H9" s="384"/>
-      <c r="I9" s="384"/>
+      <c r="F9" s="385"/>
+      <c r="G9" s="385"/>
+      <c r="H9" s="385"/>
+      <c r="I9" s="385"/>
       <c r="J9" s="75"/>
-      <c r="K9" s="385" t="s">
+      <c r="K9" s="386" t="s">
         <v>38</v>
       </c>
-      <c r="L9" s="386"/>
-      <c r="M9" s="385" t="s">
+      <c r="L9" s="387"/>
+      <c r="M9" s="386" t="s">
         <v>37</v>
       </c>
-      <c r="N9" s="383"/>
-      <c r="O9" s="383"/>
-      <c r="P9" s="383"/>
+      <c r="N9" s="384"/>
+      <c r="O9" s="384"/>
+      <c r="P9" s="384"/>
       <c r="Q9" s="74" t="s">
         <v>36</v>
       </c>
@@ -55452,11 +55434,11 @@
         <f>MAX(K13:L165)-K170</f>
         <v>1.1000000000000014</v>
       </c>
-      <c r="L176" s="382" t="s">
+      <c r="L176" s="383" t="s">
         <v>56</v>
       </c>
-      <c r="M176" s="382"/>
-      <c r="N176" s="382"/>
+      <c r="M176" s="383"/>
+      <c r="N176" s="383"/>
       <c r="O176" s="1"/>
       <c r="P176" s="1"/>
       <c r="Q176" s="1"/>
@@ -59213,28 +59195,28 @@
       <c r="B9" s="76" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="385" t="s">
+      <c r="C9" s="386" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="386"/>
-      <c r="E9" s="384" t="s">
+      <c r="D9" s="387"/>
+      <c r="E9" s="385" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="384"/>
-      <c r="G9" s="384"/>
-      <c r="H9" s="384"/>
-      <c r="I9" s="384"/>
+      <c r="F9" s="385"/>
+      <c r="G9" s="385"/>
+      <c r="H9" s="385"/>
+      <c r="I9" s="385"/>
       <c r="J9" s="75"/>
-      <c r="K9" s="385" t="s">
+      <c r="K9" s="386" t="s">
         <v>38</v>
       </c>
-      <c r="L9" s="386"/>
-      <c r="M9" s="385" t="s">
+      <c r="L9" s="387"/>
+      <c r="M9" s="386" t="s">
         <v>37</v>
       </c>
-      <c r="N9" s="383"/>
-      <c r="O9" s="383"/>
-      <c r="P9" s="383"/>
+      <c r="N9" s="384"/>
+      <c r="O9" s="384"/>
+      <c r="P9" s="384"/>
       <c r="Q9" s="74" t="s">
         <v>36</v>
       </c>
@@ -64850,7 +64832,7 @@
         <v>264</v>
       </c>
       <c r="H57" s="334" t="s">
-        <v>265</v>
+        <v>270</v>
       </c>
     </row>
     <row r="58" spans="1:8">
@@ -65223,7 +65205,7 @@
     </row>
     <row r="92" spans="1:5">
       <c r="A92" s="334" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
   </sheetData>
@@ -65470,28 +65452,28 @@
       <c r="B9" s="76" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="385" t="s">
+      <c r="C9" s="386" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="386"/>
-      <c r="E9" s="384" t="s">
+      <c r="D9" s="387"/>
+      <c r="E9" s="385" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="384"/>
-      <c r="G9" s="384"/>
-      <c r="H9" s="384"/>
-      <c r="I9" s="384"/>
+      <c r="F9" s="385"/>
+      <c r="G9" s="385"/>
+      <c r="H9" s="385"/>
+      <c r="I9" s="385"/>
       <c r="J9" s="75"/>
-      <c r="K9" s="385" t="s">
+      <c r="K9" s="386" t="s">
         <v>38</v>
       </c>
-      <c r="L9" s="386"/>
-      <c r="M9" s="385" t="s">
+      <c r="L9" s="387"/>
+      <c r="M9" s="386" t="s">
         <v>37</v>
       </c>
-      <c r="N9" s="383"/>
-      <c r="O9" s="383"/>
-      <c r="P9" s="383"/>
+      <c r="N9" s="384"/>
+      <c r="O9" s="384"/>
+      <c r="P9" s="384"/>
       <c r="Q9" s="74" t="s">
         <v>36</v>
       </c>
@@ -68308,28 +68290,28 @@
       <c r="B9" s="76" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="385" t="s">
+      <c r="C9" s="386" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="386"/>
-      <c r="E9" s="384" t="s">
+      <c r="D9" s="387"/>
+      <c r="E9" s="385" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="384"/>
-      <c r="G9" s="384"/>
-      <c r="H9" s="384"/>
-      <c r="I9" s="384"/>
+      <c r="F9" s="385"/>
+      <c r="G9" s="385"/>
+      <c r="H9" s="385"/>
+      <c r="I9" s="385"/>
       <c r="J9" s="75"/>
-      <c r="K9" s="385" t="s">
+      <c r="K9" s="386" t="s">
         <v>38</v>
       </c>
-      <c r="L9" s="386"/>
-      <c r="M9" s="385" t="s">
+      <c r="L9" s="387"/>
+      <c r="M9" s="386" t="s">
         <v>37</v>
       </c>
-      <c r="N9" s="383"/>
-      <c r="O9" s="383"/>
-      <c r="P9" s="383"/>
+      <c r="N9" s="384"/>
+      <c r="O9" s="384"/>
+      <c r="P9" s="384"/>
       <c r="Q9" s="74" t="s">
         <v>36</v>
       </c>
@@ -72253,28 +72235,28 @@
       <c r="B9" s="76" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="385" t="s">
+      <c r="C9" s="386" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="386"/>
-      <c r="E9" s="384" t="s">
+      <c r="D9" s="387"/>
+      <c r="E9" s="385" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="384"/>
-      <c r="G9" s="384"/>
-      <c r="H9" s="384"/>
-      <c r="I9" s="384"/>
+      <c r="F9" s="385"/>
+      <c r="G9" s="385"/>
+      <c r="H9" s="385"/>
+      <c r="I9" s="385"/>
       <c r="J9" s="75"/>
-      <c r="K9" s="385" t="s">
+      <c r="K9" s="386" t="s">
         <v>38</v>
       </c>
-      <c r="L9" s="386"/>
-      <c r="M9" s="385" t="s">
+      <c r="L9" s="387"/>
+      <c r="M9" s="386" t="s">
         <v>37</v>
       </c>
-      <c r="N9" s="383"/>
-      <c r="O9" s="383"/>
-      <c r="P9" s="383"/>
+      <c r="N9" s="384"/>
+      <c r="O9" s="384"/>
+      <c r="P9" s="384"/>
       <c r="Q9" s="74" t="s">
         <v>36</v>
       </c>
@@ -75938,28 +75920,28 @@
       <c r="B9" s="76" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="385" t="s">
+      <c r="C9" s="386" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="386"/>
-      <c r="E9" s="384" t="s">
+      <c r="D9" s="387"/>
+      <c r="E9" s="385" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="384"/>
-      <c r="G9" s="384"/>
-      <c r="H9" s="384"/>
-      <c r="I9" s="384"/>
+      <c r="F9" s="385"/>
+      <c r="G9" s="385"/>
+      <c r="H9" s="385"/>
+      <c r="I9" s="385"/>
       <c r="J9" s="75"/>
-      <c r="K9" s="385" t="s">
+      <c r="K9" s="386" t="s">
         <v>38</v>
       </c>
-      <c r="L9" s="386"/>
-      <c r="M9" s="385" t="s">
+      <c r="L9" s="387"/>
+      <c r="M9" s="386" t="s">
         <v>37</v>
       </c>
-      <c r="N9" s="383"/>
-      <c r="O9" s="383"/>
-      <c r="P9" s="383"/>
+      <c r="N9" s="384"/>
+      <c r="O9" s="384"/>
+      <c r="P9" s="384"/>
       <c r="Q9" s="74" t="s">
         <v>36</v>
       </c>
@@ -79551,29 +79533,29 @@
       <c r="B9" s="76" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="385" t="s">
+      <c r="C9" s="386" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="386"/>
-      <c r="E9" s="384" t="s">
+      <c r="D9" s="387"/>
+      <c r="E9" s="385" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="384"/>
-      <c r="G9" s="384"/>
-      <c r="H9" s="384"/>
-      <c r="I9" s="384"/>
+      <c r="F9" s="385"/>
+      <c r="G9" s="385"/>
+      <c r="H9" s="385"/>
+      <c r="I9" s="385"/>
       <c r="J9" s="75"/>
-      <c r="K9" s="385" t="s">
+      <c r="K9" s="386" t="s">
         <v>38</v>
       </c>
-      <c r="L9" s="386"/>
-      <c r="M9" s="385" t="s">
+      <c r="L9" s="387"/>
+      <c r="M9" s="386" t="s">
         <v>37</v>
       </c>
-      <c r="N9" s="383"/>
-      <c r="O9" s="383"/>
-      <c r="P9" s="383"/>
-      <c r="Q9" s="383"/>
+      <c r="N9" s="384"/>
+      <c r="O9" s="384"/>
+      <c r="P9" s="384"/>
+      <c r="Q9" s="384"/>
       <c r="R9" s="74" t="s">
         <v>36</v>
       </c>

</xml_diff>